<commit_message>
delete excel valuo files
</commit_message>
<xml_diff>
--- a/PYTHON/DATA_ANALYSIS/VALUO/pozemky_data.xlsx
+++ b/PYTHON/DATA_ANALYSIS/VALUO/pozemky_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,7 +535,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V-19568/2025-101</t>
+          <t>V-3408/2025-209</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -545,7 +545,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45744.49373842592</v>
+        <v>45735.375</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -553,29 +553,29 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>9833</v>
+        <v>7090</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -584,26 +584,22 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>54000000</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>DH, IZ</t>
-        </is>
-      </c>
+        <v>22000000</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>orná půda, zastavěná plocha a nádvoří</t>
+          <t>orná půda</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2372/31, 2372/34, 2372/35, 2372/36, 2372/87</t>
+          <t>493/108, 493/115</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>5492</t>
+          <t>3103</t>
         </is>
       </c>
     </row>
@@ -613,7 +609,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V-3056/2025-101</t>
+          <t>V-1370/2025-209</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -623,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45673.57884259259</v>
+        <v>45692.47313657407</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -634,26 +630,26 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>1235</v>
+        <v>411</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662496</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -662,26 +658,22 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>6490000</v>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
+        <v>3800000</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2362/77</t>
+          <t>450/4</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>5255</t>
+          <t>9246</t>
         </is>
       </c>
     </row>
@@ -691,17 +683,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>V-77826/2024-101</t>
+          <t>V-583/2025-209</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>2025</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45649.40625</v>
+        <v>45674.39223379629</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -709,29 +701,29 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>10046</v>
+        <v>28</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -740,26 +732,22 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>29900000</v>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>DH, ZMK</t>
-        </is>
-      </c>
+        <v>137200</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>jiná plocha, koryto vodního toku přirozené nebo upravené, orná půda</t>
+          <t>jiná plocha</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2370/75, 2370/76, 2477/3, 844/12</t>
+          <t>676/69</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>2976</t>
+          <t>4900</t>
         </is>
       </c>
     </row>
@@ -769,17 +757,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>V-76318/2024-101</t>
+          <t>V-431/2025-209</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>2025</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45644.39130787037</v>
+        <v>45671.49466435185</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -787,29 +775,29 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>41858</v>
+        <v>837</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662496</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -818,26 +806,22 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>54298200</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>IZ, NL/SP, OV, PS/SP, ZMK</t>
-        </is>
-      </c>
+        <v>3990000</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>koryto vodního toku přirozené nebo upravené, orná půda, ostatní komunikace</t>
+          <t>ostatní komunikace, zahrada</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>1470/176, 1477/4, 1478/11, 2350/4, 2350/5, 2350/6, 2350/7, 2351/1, 2351/3, 2351/6, 2352/21, 2352/33, 2352/34, 2352/5, 2444</t>
+          <t>236/2, 236/50, 236/51</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>1297</t>
+          <t>4767</t>
         </is>
       </c>
     </row>
@@ -847,7 +831,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>V-60292/2024-101</t>
+          <t>V-13432/2024-209</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -857,7 +841,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45581.40625</v>
+        <v>45600.375</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -865,29 +849,29 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>3681</v>
+        <v>3646</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>662496</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -896,13 +880,9 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>8950000</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>DH, ZMK</t>
-        </is>
-      </c>
+        <v>9500000</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
           <t>orná půda</t>
@@ -910,12 +890,12 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>1015/53, 835/203</t>
+          <t>553/14</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>2431</t>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -925,17 +905,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>V-57996/2024-101</t>
+          <t>V-13216/2024-209</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>2024</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45569.49055555555</v>
+        <v>45594.60856481481</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -943,29 +923,29 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>11516</v>
+        <v>3139</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662496</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Štiřín</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -974,26 +954,22 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>17484875</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>ZMK, ZMK/SV-B</t>
-        </is>
-      </c>
+        <v>21345200</v>
+      </c>
+      <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2375/6, 2375/7</t>
+          <t>379/2</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>1518</t>
+          <t>6800</t>
         </is>
       </c>
     </row>
@@ -1003,47 +979,47 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>V-52059/2024-101</t>
+          <t>V-13107/2024-209</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>2024</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45544.40625</v>
+        <v>45590.35416666666</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Potvrzení o nabytí vlastnictví předmětu dražby (zák. č. 26/2000 Sb.)</t>
+          <t>Smlouva kupní</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>650</v>
+        <v>19</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Krč</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>727598</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Krč</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1052,26 +1028,22 @@
         </is>
       </c>
       <c r="N8" t="n">
-        <v>770000</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>ZP</t>
-        </is>
-      </c>
+        <v>76000</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>jiná plocha, zeleň</t>
+          <t>ostatní komunikace</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2209/17, 2216/2</t>
+          <t>746/4</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>1185</t>
+          <t>4000</t>
         </is>
       </c>
     </row>
@@ -1081,17 +1053,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>V-46186/2024-101</t>
+          <t>V-11871/2024-209</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>2024</v>
       </c>
       <c r="D9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>45513.46150462963</v>
+        <v>45566.45238425926</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1099,29 +1071,29 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
-        <v>914</v>
+        <v>846</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1130,13 +1102,9 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>6000000</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>5000000</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
           <t>zahrada</t>
@@ -1144,12 +1112,12 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>741</t>
+          <t>639/28, 639/6</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>6565</t>
+          <t>5910</t>
         </is>
       </c>
     </row>
@@ -1159,7 +1127,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>V-32174/2024-101</t>
+          <t>V-11472/2024-209</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1169,7 +1137,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45447.36206018519</v>
+        <v>45558.3950462963</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1177,29 +1145,29 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>6461</v>
+        <v>1008</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1208,26 +1176,22 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>50000000</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>8200000</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2349/15</t>
+          <t>725/28</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>7739</t>
+          <t>8135</t>
         </is>
       </c>
     </row>
@@ -1237,17 +1201,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>V-24009/2024-101</t>
+          <t>V-7107/2024-201</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>2024</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>45407.41380787037</v>
+        <v>45538.375</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1258,26 +1222,26 @@
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>914</v>
+        <v>697</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1286,26 +1250,22 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>6800000</v>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>4490000</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>zahrada</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>741</t>
+          <t>160/259</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>7440</t>
+          <t>6442</t>
         </is>
       </c>
     </row>
@@ -1315,17 +1275,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>V-20893/2024-101</t>
+          <t>V-10462/2024-209</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>2024</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>45393.51142361111</v>
+        <v>45533.45623842593</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1333,29 +1293,29 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" t="n">
-        <v>1235</v>
+        <v>576</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1364,26 +1324,22 @@
         </is>
       </c>
       <c r="N12" t="n">
-        <v>6490000</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
+        <v>2900000</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2362/77</t>
+          <t>255/8, 722/12</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>5255</t>
+          <t>5035</t>
         </is>
       </c>
     </row>
@@ -1393,17 +1349,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>V-16230/2024-101</t>
+          <t>V-10282/2024-209</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>2024</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>45371.5595949074</v>
+        <v>45530.41327546296</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1411,29 +1367,29 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" t="n">
-        <v>25</v>
+        <v>7735</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1442,26 +1398,22 @@
         </is>
       </c>
       <c r="N13" t="n">
-        <v>49000</v>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
+        <v>13496250</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>orná půda, zahrada</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2362/66</t>
+          <t>285/18, 285/30, 285/31</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>1745</t>
         </is>
       </c>
     </row>
@@ -1471,47 +1423,47 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>V-11441/2024-101</t>
+          <t>V-9889/2024-209</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>2024</v>
       </c>
       <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45519.53748842593</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Smlouva kupní</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
         <v>3</v>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>45349.47018518519</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Smlouva kupní</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>25</v>
-      </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1520,26 +1472,22 @@
         </is>
       </c>
       <c r="N14" t="n">
-        <v>100000</v>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
+        <v>3000</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2362/66</t>
+          <t>802/24</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
@@ -1549,17 +1497,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>V-8713/2024-101</t>
+          <t>V-9676/2024-209</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>2024</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>45336.44564814815</v>
+        <v>45516.61221064815</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1570,26 +1518,26 @@
         <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>25</v>
+        <v>1365</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1598,26 +1546,22 @@
         </is>
       </c>
       <c r="N15" t="n">
-        <v>80000</v>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
+        <v>6780500</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2362/66</t>
+          <t>874/16</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>3200</t>
+          <t>4967</t>
         </is>
       </c>
     </row>
@@ -1627,17 +1571,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>V-345/2024-101</t>
+          <t>V-7784/2024-209</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>2024</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>45294.63649305556</v>
+        <v>45471.37259259259</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1645,29 +1589,29 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>986</v>
+        <v>1010</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1676,26 +1620,22 @@
         </is>
       </c>
       <c r="N16" t="n">
-        <v>8929970</v>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>8250000</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>jiná plocha</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>826/4</t>
+          <t>725/2</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>9057</t>
+          <t>8168</t>
         </is>
       </c>
     </row>
@@ -1705,17 +1645,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>V-47590/2023-101</t>
+          <t>V-7112/2024-209</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>45177.4828587963</v>
+        <v>45460.37694444445</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1726,26 +1666,26 @@
         <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>41</v>
+        <v>1259</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1754,26 +1694,22 @@
         </is>
       </c>
       <c r="N17" t="n">
-        <v>115000</v>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>8700000</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>trvalý travní porost</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2110/38</t>
+          <t>874/101</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>6910</t>
         </is>
       </c>
     </row>
@@ -1783,17 +1719,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>V-45061/2023-101</t>
+          <t>V-7063/2024-209</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>45163.48635416666</v>
+        <v>45457.37336805555</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1804,26 +1740,26 @@
         <v>2</v>
       </c>
       <c r="H18" t="n">
-        <v>957</v>
+        <v>432</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Krč</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>727598</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Krč</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1832,26 +1768,22 @@
         </is>
       </c>
       <c r="N18" t="n">
-        <v>5685000</v>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>VV</t>
-        </is>
-      </c>
+        <v>1450000</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>silnice, zahrada</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2583/1, 3315/7</t>
+          <t>664/2, 664/27</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>3356</t>
         </is>
       </c>
     </row>
@@ -1861,17 +1793,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>V-42230/2023-101</t>
+          <t>V-7032/2024-209</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D19" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>45147.62395833333</v>
+        <v>45456.48310185185</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1879,29 +1811,29 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H19" t="n">
-        <v>6210</v>
+        <v>4142</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662500</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Těptín</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1910,26 +1842,26 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>43000000</v>
+        <v>6200000</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>ZMK</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>manipulační plocha</t>
+          <t>neplodná půda, ostatní komunikace, zahrada</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>1433/10, 1433/11, 1433/12, 1433/13</t>
+          <t>619/17, 619/2, 619/89, 619/98, 619/99, 621/3</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>6924</t>
+          <t>1497</t>
         </is>
       </c>
     </row>
@@ -1939,17 +1871,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>V-38642/2023-101</t>
+          <t>V-4514/2024-201</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D20" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>45128.3612037037</v>
+        <v>45447.55001157407</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1957,29 +1889,29 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>3794</v>
+        <v>1254</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1988,26 +1920,22 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>22531700</v>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>VN-D</t>
-        </is>
-      </c>
+        <v>1600000</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2368/29, 2370/11</t>
+          <t>1119/2</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>5939</t>
+          <t>1276</t>
         </is>
       </c>
     </row>
@@ -2017,17 +1945,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>V-36815/2023-101</t>
+          <t>V-5555/2024-209</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>45118.99244212963</v>
+        <v>45427.48658564815</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2035,29 +1963,29 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>2104</v>
+        <v>51</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -2066,26 +1994,22 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>5700000</v>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>122400</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>jiná plocha, zahrada</t>
+          <t>neplodná půda</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>1158, 1159</t>
+          <t>511/4</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>2709</t>
+          <t>2400</t>
         </is>
       </c>
     </row>
@@ -2095,17 +2019,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>V-7793/2023-101</t>
+          <t>V-3805/2024-201</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>44970.34607638889</v>
+        <v>45425.40150462963</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2113,29 +2037,29 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>4130</v>
+        <v>1228</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2144,26 +2068,22 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>18174800</v>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>DH, ZMK</t>
-        </is>
-      </c>
+        <v>6500000</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t>manipulační plocha, ostatní komunikace, silnice</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>879/16, 879/17, 879/4, 880/17</t>
+          <t>160/123</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>4401</t>
+          <t>5293</t>
         </is>
       </c>
     </row>
@@ -2173,17 +2093,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>V-1609/2023-101</t>
+          <t>V-5025/2024-209</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44936.55086805556</v>
+        <v>45414.35416666666</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2194,26 +2114,26 @@
         <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>10203</v>
+        <v>117</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2222,26 +2142,22 @@
         </is>
       </c>
       <c r="N23" t="n">
-        <v>12000000</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>OP/NL</t>
-        </is>
-      </c>
+        <v>250000</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>jiná plocha</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2357/44</t>
+          <t>1240/34</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>1176</t>
+          <t>2137</t>
         </is>
       </c>
     </row>
@@ -2251,17 +2167,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>V-39047/2022-101</t>
+          <t>V-4446/2024-209</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>44735.54371527778</v>
+        <v>45401.36630787037</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2269,29 +2185,29 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" t="n">
-        <v>14842</v>
+        <v>1125</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -2300,26 +2216,22 @@
         </is>
       </c>
       <c r="N24" t="n">
-        <v>30400000</v>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>PS, ZMK</t>
-        </is>
-      </c>
+        <v>6700000</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>orná půda, ovocný sad</t>
+          <t>ostatní komunikace, trvalý travní porost</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>1872, 2366/34</t>
+          <t>141/179, 141/259</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>2048</t>
+          <t>5956</t>
         </is>
       </c>
     </row>
@@ -2329,17 +2241,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>V-4586/2022-101</t>
+          <t>V-860/2024-201</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="D25" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44582.4278125</v>
+        <v>45323.54754629629</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2350,26 +2262,26 @@
         <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>4128</v>
+        <v>1489</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2378,26 +2290,22 @@
         </is>
       </c>
       <c r="N25" t="n">
-        <v>16512000</v>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>DH</t>
-        </is>
-      </c>
+        <v>6000000</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
-          <t>jiná plocha</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>844/8</t>
+          <t>160/167</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>4030</t>
         </is>
       </c>
     </row>
@@ -2407,17 +2315,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>V-90297/2021-101</t>
+          <t>V-606/2024-201</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D26" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>44531.47324074074</v>
+        <v>45315.375</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2425,29 +2333,29 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>6874</v>
+        <v>1555</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2456,26 +2364,22 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>34356252</v>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>DH</t>
-        </is>
-      </c>
+        <v>8200000</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2372/5, 2372/88</t>
+          <t>630/20</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>4998</t>
+          <t>5273</t>
         </is>
       </c>
     </row>
@@ -2485,17 +2389,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>V-89035/2021-101</t>
+          <t>V-14734/2023-209</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D27" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>44526.36560185185</v>
+        <v>45282.63912037037</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2503,29 +2407,29 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>2245</v>
+        <v>1501</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2534,26 +2438,22 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>8500000</v>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>8250000</v>
+      </c>
+      <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>koryto vodního toku přirozené nebo upravené, orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2368/16, 2368/30, 2477/7</t>
+          <t>761/9</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>3786</t>
+          <t>5496</t>
         </is>
       </c>
     </row>
@@ -2563,17 +2463,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>V-85678/2021-101</t>
+          <t>V-14475/2023-209</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D28" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>44515.36931712963</v>
+        <v>45279.48119212963</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2581,29 +2481,29 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>6509</v>
+        <v>930</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2612,26 +2512,22 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>16980000</v>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>6000000</v>
+      </c>
+      <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>646/48</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>2609</t>
+          <t>6452</t>
         </is>
       </c>
     </row>
@@ -2641,17 +2537,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>V-82681/2021-101</t>
+          <t>V-14272/2023-209</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D29" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>44503.34978009259</v>
+        <v>45274.43002314815</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2662,26 +2558,26 @@
         <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>584</v>
+        <v>1150</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>728390</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2690,26 +2586,22 @@
         </is>
       </c>
       <c r="N29" t="n">
-        <v>1868800</v>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>IZ</t>
-        </is>
-      </c>
+        <v>5500000</v>
+      </c>
+      <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t>jiná plocha</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>675/20</t>
+          <t>1072/6</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>3200</t>
+          <t>4783</t>
         </is>
       </c>
     </row>
@@ -2719,17 +2611,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>V-81373/2021-101</t>
+          <t>V-9138/2023-201</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D30" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>44496.40277777778</v>
+        <v>45268.375</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -2737,29 +2629,29 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>6434</v>
+        <v>1014</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -2768,26 +2660,22 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>15855000</v>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>3200000</v>
+      </c>
+      <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>618/9</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>2464</t>
+          <t>3156</t>
         </is>
       </c>
     </row>
@@ -2797,17 +2685,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>V-78317/2021-101</t>
+          <t>V-13792/2023-209</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D31" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>44487.36446759259</v>
+        <v>45265.55150462963</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2815,29 +2703,29 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>6413</v>
+        <v>1182</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -2846,26 +2734,22 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>15540000</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>9300000</v>
+      </c>
+      <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>675/5</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>2423</t>
+          <t>7868</t>
         </is>
       </c>
     </row>
@@ -2875,17 +2759,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>V-71005/2021-101</t>
+          <t>V-8798/2023-201</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>44456.37630787037</v>
+        <v>45257.6069212963</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -2893,29 +2777,29 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>6781</v>
+        <v>1014</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -2924,26 +2808,22 @@
         </is>
       </c>
       <c r="N32" t="n">
-        <v>21060000</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>3200000</v>
+      </c>
+      <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>618/8</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>3106</t>
+          <t>3156</t>
         </is>
       </c>
     </row>
@@ -2953,17 +2833,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>V-69431/2021-101</t>
+          <t>V-12592/2023-209</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>44452.4024074074</v>
+        <v>45238.36049768519</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2971,29 +2851,29 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>6460</v>
+        <v>1334</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -3002,26 +2882,22 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>16245000</v>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>9350000</v>
+      </c>
+      <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>874/60</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>2515</t>
+          <t>7009</t>
         </is>
       </c>
     </row>
@@ -3031,17 +2907,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>V-69426/2021-101</t>
+          <t>V-12419/2023-209</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D34" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>44452.39978009259</v>
+        <v>45233.44167824074</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -3049,29 +2925,29 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>8164</v>
+        <v>1000</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -3080,26 +2956,22 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>41805000</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>2500000</v>
+      </c>
+      <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>418/48</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>5121</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3109,17 +2981,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>V-56400/2021-101</t>
+          <t>V-11949/2023-209</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D35" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>44399.5066087963</v>
+        <v>45223.60994212963</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -3127,29 +2999,29 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>14842</v>
+        <v>1008</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -3158,26 +3030,22 @@
         </is>
       </c>
       <c r="N35" t="n">
-        <v>35000000</v>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>PS, ZMK</t>
-        </is>
-      </c>
+        <v>8300000</v>
+      </c>
+      <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t>orná půda, ovocný sad</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>1872, 2366/34</t>
+          <t>874/85</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>2358</t>
+          <t>8234</t>
         </is>
       </c>
     </row>
@@ -3187,17 +3055,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>V-56243/2021-101</t>
+          <t>V-10840/2023-209</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>44399.37063657407</v>
+        <v>45198.40049768519</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -3208,26 +3076,26 @@
         <v>2</v>
       </c>
       <c r="H36" t="n">
-        <v>39</v>
+        <v>21485</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>728390</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Libuš</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3236,26 +3104,22 @@
         </is>
       </c>
       <c r="N36" t="n">
-        <v>253500</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>30950000</v>
+      </c>
+      <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>orná půda</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>318/4, 318/6</t>
+          <t>803/70, 803/85</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>6500</t>
+          <t>1441</t>
         </is>
       </c>
     </row>
@@ -3265,17 +3129,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>V-51944/2021-101</t>
+          <t>V-9091/2023-209</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D37" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>44379.52472222222</v>
+        <v>45153.37292824074</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -3283,29 +3147,29 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>6354</v>
+        <v>246</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -3314,26 +3178,22 @@
         </is>
       </c>
       <c r="N37" t="n">
-        <v>11063400</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>432000</v>
+      </c>
+      <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t>lesní pozemek</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>2340/2</t>
+          <t>234/4</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>1756</t>
         </is>
       </c>
     </row>
@@ -3343,17 +3203,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>V-35676/2021-101</t>
+          <t>V-8714/2023-209</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D38" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>44328.36924768519</v>
+        <v>45142.4522337963</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -3361,29 +3221,29 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H38" t="n">
-        <v>6453</v>
+        <v>1662</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -3392,26 +3252,22 @@
         </is>
       </c>
       <c r="N38" t="n">
-        <v>16140000</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>4000000</v>
+      </c>
+      <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>414/48, 414/49</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>2501</t>
+          <t>2407</t>
         </is>
       </c>
     </row>
@@ -3421,47 +3277,47 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>V-33534/2021-101</t>
+          <t>V-4676/2023-201</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>44320.56076388889</v>
+        <v>45103.4030787037</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Smlouva kupní, Smlouva o zřízení věcného břemene - bezúplatná</t>
+          <t>Smlouva kupní</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
-        <v>2702</v>
+        <v>1266</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Benešov</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>737054</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Pyšely</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -3470,26 +3326,22 @@
         </is>
       </c>
       <c r="N39" t="n">
-        <v>12000000</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>4000000</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>2356/212</t>
+          <t>160/190</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>4441</t>
+          <t>3160</t>
         </is>
       </c>
     </row>
@@ -3499,17 +3351,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>V-23894/2021-101</t>
+          <t>V-4962/2023-209</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>44285.48607638889</v>
+        <v>45050.46203703704</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -3517,29 +3369,29 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>6267</v>
+        <v>1191</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -3548,26 +3400,22 @@
         </is>
       </c>
       <c r="N40" t="n">
-        <v>13350000</v>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>11500000</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr">
         <is>
-          <t>ostatní komunikace</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>48/1</t>
+          <t>671/123</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>2130</t>
+          <t>9656</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3425,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>V-22856/2021-101</t>
+          <t>V-2860/2023-209</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D41" t="n">
         <v>4</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>44280.55900462963</v>
+        <v>44999.52289351852</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -3598,26 +3446,26 @@
         <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>825</v>
+        <v>2481</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -3626,26 +3474,22 @@
         </is>
       </c>
       <c r="N41" t="n">
-        <v>2800000</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>9000000</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t>manipulační plocha</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>880/15</t>
+          <t>634/3</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>3394</t>
+          <t>3628</t>
         </is>
       </c>
     </row>
@@ -3655,17 +3499,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>V-73602/2020-101</t>
+          <t>V-2373/2023-209</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="D42" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>44167.57769675926</v>
+        <v>44987.50519675926</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -3673,29 +3517,29 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>4365</v>
+        <v>1214</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>720984</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Písnice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -3704,26 +3548,22 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>8387000</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>VN</t>
-        </is>
-      </c>
+        <v>7540000</v>
+      </c>
+      <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t>manipulační plocha</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>669/11, 669/12, 669/13, 669/14, 669/15, 669/16, 669/17, 669/8</t>
+          <t>418/30</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>1921</t>
+          <t>6211</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3573,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>V-64834/2020-101</t>
+          <t>V-2056/2023-209</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="D43" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>44137.45591435185</v>
+        <v>44980.35416666666</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -3751,29 +3591,29 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H43" t="n">
-        <v>1215</v>
+        <v>634</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -3782,26 +3622,22 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
+        <v>4300000</v>
+      </c>
+      <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t>orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>2362/15</t>
+          <t>204/19</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>1646</t>
+          <t>6782</t>
         </is>
       </c>
     </row>
@@ -3811,17 +3647,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>V-55881/2020-101</t>
+          <t>V-1509/2023-209</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="D44" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>44097.45791666667</v>
+        <v>44966.41483796296</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -3832,26 +3668,26 @@
         <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>3251</v>
+        <v>102</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -3860,26 +3696,22 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>11400000</v>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>VN-C</t>
-        </is>
-      </c>
+        <v>306000</v>
+      </c>
+      <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t>jiná plocha</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>2377/23</t>
+          <t>234/4</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>3507</t>
+          <t>3000</t>
         </is>
       </c>
     </row>
@@ -3889,17 +3721,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>V-28713/2020-101</t>
+          <t>V-389/2023-209</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="D45" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>43976.38417824074</v>
+        <v>44938.44333333334</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -3907,29 +3739,29 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>7403</v>
+        <v>200</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>662445</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Ládví</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -3938,13 +3770,9 @@
         </is>
       </c>
       <c r="N45" t="n">
-        <v>24800050</v>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>DH, IZ, ZMK</t>
-        </is>
-      </c>
+        <v>990000</v>
+      </c>
+      <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
           <t>orná půda</t>
@@ -3952,12 +3780,12 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>2370/28, 2370/41, 2370/42, 2370/47</t>
+          <t>432/25</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>3350</t>
+          <t>4950</t>
         </is>
       </c>
     </row>
@@ -3967,17 +3795,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>V-24337/2020-101</t>
+          <t>V-14475/2022-209</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D46" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>43955.53079861111</v>
+        <v>44868.47243055556</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -3985,29 +3813,29 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>2245</v>
+        <v>2287</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
@@ -4016,26 +3844,26 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>7500000</v>
+        <v>14000000</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>ZMK</t>
+          <t>SV</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>koryto vodního toku přirozené nebo upravené, orná půda</t>
+          <t>zahrada</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>2368/16, 2368/2, 2477/7</t>
+          <t>626/1</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>3341</t>
+          <t>6122</t>
         </is>
       </c>
     </row>
@@ -4045,17 +3873,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>V-1024/2020-101</t>
+          <t>V-7911/2022-209</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>43839.4258912037</v>
+        <v>44719.46099537037</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -4066,26 +3894,26 @@
         <v>1</v>
       </c>
       <c r="H47" t="n">
-        <v>914</v>
+        <v>113</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
@@ -4094,26 +3922,22 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>4900000</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>OV</t>
-        </is>
-      </c>
+        <v>500000</v>
+      </c>
+      <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr">
         <is>
-          <t>zahrada</t>
+          <t>trvalý travní porost</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>741</t>
+          <t>922/8</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>5361</t>
+          <t>4425</t>
         </is>
       </c>
     </row>
@@ -4123,17 +3947,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>V-85048/2019-101</t>
+          <t>V-7532/2022-209</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>43822.54815972222</v>
+        <v>44711.59616898148</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -4144,26 +3968,26 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>1602</v>
+        <v>1617</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Praha-východ</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>728314</t>
+          <t>759431</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Kunratice</t>
+          <t>Sulice</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -4172,13 +3996,9 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>3204000</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>ZMK</t>
-        </is>
-      </c>
+        <v>9400000</v>
+      </c>
+      <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr">
         <is>
           <t>orná půda</t>
@@ -4186,12 +4006,390 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>2353/15</t>
+          <t>774/6</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>5813</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>V-3524/2022-209</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D49" t="n">
+        <v>6</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>44631.44509259259</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Smlouva kupní</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>9</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4295</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Praha-východ</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>759431</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>12600000</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>OV</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>ostatní komunikace, trvalý travní porost, zahrada</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>1268/13, 1268/8, 1270/8, 1270/9, 1285, 1296</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>2934</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>V-3520/2022-209</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D50" t="n">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>44631.4407175926</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Smlouva kupní</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>7</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3483</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Praha-východ</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>759431</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>32250000</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>OV</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>ostatní komunikace, trvalý travní porost</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>1268/10, 1268/13, 1268/8, 1269/7, 1270/8, 1270/9, 1296</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>9259</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>V-3065/2022-209</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>44623.37024305556</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Smlouva kupní</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>2</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1329</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Praha-východ</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>759431</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>11000000</v>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>zahrada</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>874/14</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>8277</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>V-903/2022-209</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>44581.35416666666</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Smlouva kupní</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1066</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Praha-východ</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>759431</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>8390000</v>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>orná půda</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>418/32</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>7871</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>V-20021/2021-209</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>44544.56427083333</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Smlouva kupní</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1365</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Praha-východ</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>759431</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Sulice</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>parcela</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>11800000</v>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>orná půda</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>874/16</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>8645</t>
         </is>
       </c>
     </row>

</xml_diff>